<commit_message>
git status~BIGGER SIGH~git status
</commit_message>
<xml_diff>
--- a/data/xlsx_edit/physrost16.xlsx
+++ b/data/xlsx_edit/physrost16.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2343" uniqueCount="815">
   <si>
     <t xml:space="preserve">Institution</t>
   </si>
@@ -2757,10 +2757,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P752"/>
+  <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A625" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A643" activeCellId="0" sqref="A643"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2814,7 +2814,7 @@
       <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0"/>
+      <c r="P1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -21491,27 +21491,45 @@
       </c>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A643" s="1" t="s">
+        <v>699</v>
+      </c>
       <c r="B643" s="1" t="s">
         <v>683</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A644" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B644" s="1" t="s">
         <v>683</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="F644" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="G644" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="H644" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I644" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M644" s="1" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A645" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B645" s="1" t="s">
         <v>683</v>
@@ -21520,91 +21538,91 @@
         <v>23</v>
       </c>
       <c r="F645" s="1" t="n">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="G645" s="1" t="n">
-        <v>16</v>
+        <v>152</v>
       </c>
       <c r="H645" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I645" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M645" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A646" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B646" s="1" t="s">
         <v>683</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F646" s="1" t="n">
-        <v>64</v>
+        <v>388</v>
       </c>
       <c r="G646" s="1" t="n">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="H646" s="1" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="I646" s="1" t="n">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="J646" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="K646" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="L646" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="M646" s="1" t="n">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="N646" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O646" s="1" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A647" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B647" s="1" t="s">
-        <v>683</v>
+        <v>704</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F647" s="1" t="n">
-        <v>388</v>
+        <v>132</v>
       </c>
       <c r="G647" s="1" t="n">
-        <v>145</v>
+        <v>255</v>
       </c>
       <c r="H647" s="1" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="I647" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="J647" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="K647" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="L647" s="1" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="M647" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="N647" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O647" s="1" t="n">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A648" s="1" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="B648" s="1" t="s">
         <v>704</v>
@@ -21613,24 +21631,24 @@
         <v>23</v>
       </c>
       <c r="F648" s="1" t="n">
-        <v>132</v>
+        <v>292</v>
       </c>
       <c r="G648" s="1" t="n">
-        <v>255</v>
+        <v>430</v>
       </c>
       <c r="H648" s="1" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="I648" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="M648" s="1" t="n">
         <v>6</v>
-      </c>
-      <c r="M648" s="1" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A649" s="1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B649" s="1" t="s">
         <v>704</v>
@@ -21639,61 +21657,61 @@
         <v>23</v>
       </c>
       <c r="F649" s="1" t="n">
-        <v>292</v>
+        <v>89</v>
       </c>
       <c r="G649" s="1" t="n">
-        <v>430</v>
+        <v>42</v>
       </c>
       <c r="H649" s="1" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I649" s="1" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="M649" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A650" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B650" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C650" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F650" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="G650" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="H650" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="I650" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="M650" s="1" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A651" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B651" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
+      </c>
+      <c r="F651" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="G651" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="H651" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I651" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="M651" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A652" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B652" s="1" t="s">
         <v>704</v>
@@ -21702,102 +21720,102 @@
         <v>23</v>
       </c>
       <c r="F652" s="1" t="n">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="G652" s="1" t="n">
-        <v>109</v>
+        <v>30</v>
       </c>
       <c r="H652" s="1" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I652" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M652" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A653" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B653" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F653" s="1" t="n">
-        <v>140</v>
+        <v>4837</v>
       </c>
       <c r="G653" s="1" t="n">
-        <v>30</v>
+        <v>361</v>
       </c>
       <c r="H653" s="1" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="I653" s="1" t="n">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="J653" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="K653" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="L653" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="M653" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
+      </c>
+      <c r="N653" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O653" s="1" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A654" s="1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B654" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F654" s="1" t="n">
-        <v>4837</v>
-      </c>
-      <c r="G654" s="1" t="n">
-        <v>361</v>
-      </c>
-      <c r="H654" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="I654" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="J654" s="1" t="n">
-        <v>116</v>
-      </c>
-      <c r="K654" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="L654" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="M654" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="N654" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O654" s="1" t="n">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A655" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B655" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
+      </c>
+      <c r="F655" s="1" t="n">
+        <v>1019</v>
+      </c>
+      <c r="G655" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="H655" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I655" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="M655" s="1" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A656" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B656" s="1" t="s">
         <v>704</v>
@@ -21806,24 +21824,24 @@
         <v>23</v>
       </c>
       <c r="F656" s="1" t="n">
-        <v>1019</v>
+        <v>49</v>
       </c>
       <c r="G656" s="1" t="n">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="H656" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I656" s="1" t="n">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="M656" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A657" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B657" s="1" t="s">
         <v>704</v>
@@ -21831,132 +21849,132 @@
       <c r="C657" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F657" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="G657" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="H657" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I657" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M657" s="1" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A658" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B658" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C658" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="F658" s="1" t="n">
+        <v>1613</v>
+      </c>
+      <c r="G658" s="1" t="n">
+        <v>3825</v>
+      </c>
+      <c r="H658" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="I658" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="J658" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="K658" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="L658" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="M658" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="N658" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O658" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A659" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B659" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C659" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F659" s="1" t="n">
-        <v>1613</v>
-      </c>
-      <c r="G659" s="1" t="n">
-        <v>3825</v>
-      </c>
-      <c r="H659" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="I659" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="J659" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="K659" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="L659" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="M659" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="N659" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="O659" s="1" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A660" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B660" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C660" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="D660" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F660" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="G660" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H660" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="I660" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="J660" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="K660" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="L660" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="M660" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="N660" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="O660" s="1" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A661" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B661" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C661" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D661" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F661" s="1" t="n">
-        <v>512</v>
+        <v>365</v>
       </c>
       <c r="G661" s="1" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H661" s="1" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="I661" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="J661" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="K661" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="L661" s="1" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="M661" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="N661" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="O661" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A662" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B662" s="1" t="s">
         <v>704</v>
@@ -21965,248 +21983,248 @@
         <v>23</v>
       </c>
       <c r="F662" s="1" t="n">
-        <v>365</v>
+        <v>449</v>
       </c>
       <c r="G662" s="1" t="n">
-        <v>32</v>
+        <v>488</v>
       </c>
       <c r="H662" s="1" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I662" s="1" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="M662" s="1" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A663" s="1" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B663" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C663" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F663" s="1" t="n">
-        <v>449</v>
+        <v>411</v>
       </c>
       <c r="G663" s="1" t="n">
-        <v>488</v>
+        <v>27</v>
       </c>
       <c r="H663" s="1" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I663" s="1" t="n">
-        <v>20</v>
+        <v>7</v>
+      </c>
+      <c r="J663" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="K663" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L663" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="M663" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="N663" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O663" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A664" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B664" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C664" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F664" s="1" t="n">
-        <v>411</v>
-      </c>
-      <c r="G664" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="H664" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="I664" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="J664" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="K664" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="L664" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M664" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="N664" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="O664" s="1" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A665" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B665" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+      <c r="F665" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="G665" s="1" t="n">
+        <v>1098</v>
+      </c>
+      <c r="H665" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="I665" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="J665" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K665" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L665" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M665" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N665" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A666" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B666" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F666" s="1" t="n">
-        <v>245</v>
+        <v>480</v>
       </c>
       <c r="G666" s="1" t="n">
-        <v>1098</v>
+        <v>174</v>
       </c>
       <c r="H666" s="1" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="I666" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="J666" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K666" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L666" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M666" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N666" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A667" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B667" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="D667" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F667" s="1" t="n">
-        <v>480</v>
+        <v>3745</v>
       </c>
       <c r="G667" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H667" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="I667" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="J667" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="H667" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="I667" s="1" t="n">
-        <v>4</v>
+      <c r="K667" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="L667" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="M667" s="1" t="n">
-        <v>6</v>
+        <v>26</v>
+      </c>
+      <c r="N667" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O667" s="1" t="n">
+        <v>29</v>
       </c>
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A668" s="1" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B668" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D668" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F668" s="1" t="n">
-        <v>3745</v>
+        <v>257</v>
       </c>
       <c r="G668" s="1" t="n">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="H668" s="1" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="I668" s="1" t="n">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="J668" s="1" t="n">
-        <v>174</v>
+        <v>50</v>
       </c>
       <c r="K668" s="1" t="n">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="L668" s="1" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="M668" s="1" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="N668" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="O668" s="1" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A669" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B669" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F669" s="1" t="n">
-        <v>257</v>
+        <v>517</v>
       </c>
       <c r="G669" s="1" t="n">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="H669" s="1" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="I669" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="J669" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="K669" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="L669" s="1" t="n">
-        <v>42</v>
+        <v>1</v>
       </c>
       <c r="M669" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="N669" s="1" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B670" s="1" t="s">
         <v>704</v>
@@ -22214,80 +22232,80 @@
       <c r="C670" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F670" s="1" t="n">
-        <v>517</v>
-      </c>
-      <c r="G670" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="H670" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I670" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M670" s="1" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A671" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B671" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="D671" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F671" s="1" t="n">
+        <v>413</v>
+      </c>
+      <c r="G671" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H671" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I671" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="J671" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="K671" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="L671" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="M671" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="N671" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O671" s="1" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A672" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B672" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D672" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F672" s="1" t="n">
-        <v>413</v>
+        <v>44</v>
       </c>
       <c r="G672" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H672" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I672" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="J672" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="K672" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="L672" s="1" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M672" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="N672" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O672" s="1" t="n">
-        <v>6</v>
-      </c>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A673" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B673" s="1" t="s">
         <v>704</v>
@@ -22295,74 +22313,89 @@
       <c r="C673" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F673" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="G673" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H673" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I673" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="M673" s="1" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A674" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B674" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C674" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+      <c r="F674" s="1" t="n">
+        <v>3084</v>
+      </c>
+      <c r="G674" s="1" t="n">
+        <v>352</v>
+      </c>
+      <c r="H674" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="I674" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="J674" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="K674" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L674" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="M674" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="N674" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A675" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B675" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C675" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F675" s="1" t="n">
+        <v>1546</v>
+      </c>
+      <c r="G675" s="1" t="n">
+        <v>656</v>
+      </c>
+      <c r="H675" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="I675" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="F675" s="1" t="n">
-        <v>3084</v>
-      </c>
-      <c r="G675" s="1" t="n">
-        <v>352</v>
-      </c>
-      <c r="H675" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="I675" s="1" t="n">
-        <v>23</v>
-      </c>
       <c r="J675" s="1" t="n">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="K675" s="1" t="n">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="L675" s="1" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M675" s="1" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="N675" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O675" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A676" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B676" s="1" t="s">
         <v>704</v>
@@ -22370,40 +22403,28 @@
       <c r="C676" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F676" s="1" t="n">
-        <v>1546</v>
-      </c>
-      <c r="G676" s="1" t="n">
-        <v>656</v>
-      </c>
-      <c r="H676" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="I676" s="1" t="n">
-        <v>38</v>
-      </c>
       <c r="J676" s="1" t="n">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="K676" s="1" t="n">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="L676" s="1" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="M676" s="1" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="N676" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O676" s="1" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A677" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B677" s="1" t="s">
         <v>704</v>
@@ -22411,197 +22432,194 @@
       <c r="C677" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D677" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F677" s="1" t="n">
+        <v>4734</v>
+      </c>
+      <c r="G677" s="1" t="n">
+        <v>1131</v>
+      </c>
+      <c r="H677" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="I677" s="1" t="n">
+        <v>205</v>
+      </c>
       <c r="J677" s="1" t="n">
-        <v>53</v>
+        <v>206</v>
       </c>
       <c r="K677" s="1" t="n">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="L677" s="1" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="M677" s="1" t="n">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="N677" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O677" s="1" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A678" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B678" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C678" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D678" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F678" s="1" t="n">
-        <v>4734</v>
+        <v>1460</v>
       </c>
       <c r="G678" s="1" t="n">
-        <v>1131</v>
+        <v>1636</v>
       </c>
       <c r="H678" s="1" t="n">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="I678" s="1" t="n">
-        <v>205</v>
+        <v>79</v>
       </c>
       <c r="J678" s="1" t="n">
-        <v>206</v>
+        <v>19</v>
       </c>
       <c r="K678" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="L678" s="1" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="M678" s="1" t="n">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="N678" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="O678" s="1" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A679" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B679" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C679" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F679" s="1" t="n">
-        <v>1460</v>
-      </c>
-      <c r="G679" s="1" t="n">
-        <v>1636</v>
-      </c>
-      <c r="H679" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="I679" s="1" t="n">
-        <v>79</v>
-      </c>
-      <c r="J679" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="K679" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="M679" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="N679" s="1" t="n">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A680" s="1" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B680" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="F680" s="1" t="n">
+        <v>1558</v>
+      </c>
+      <c r="G680" s="1" t="n">
+        <v>854</v>
+      </c>
+      <c r="H680" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="I680" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="J680" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="K680" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="L680" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="M680" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="N680" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A681" s="1" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B681" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C681" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="F681" s="1" t="n">
-        <v>1558</v>
+        <v>2029</v>
       </c>
       <c r="G681" s="1" t="n">
-        <v>854</v>
+        <v>829</v>
       </c>
       <c r="H681" s="1" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="I681" s="1" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="J681" s="1" t="n">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="K681" s="1" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="L681" s="1" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M681" s="1" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N681" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="O681" s="1" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A682" s="1" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B682" s="1" t="s">
         <v>704</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F682" s="1" t="n">
-        <v>2029</v>
+        <v>143</v>
       </c>
       <c r="G682" s="1" t="n">
-        <v>829</v>
+        <v>146</v>
       </c>
       <c r="H682" s="1" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="I682" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="J682" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="K682" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="L682" s="1" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="M682" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="N682" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="O682" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="1" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B683" s="1" t="s">
         <v>704</v>
@@ -22610,50 +22628,65 @@
         <v>23</v>
       </c>
       <c r="F683" s="1" t="n">
-        <v>143</v>
+        <v>295</v>
       </c>
       <c r="G683" s="1" t="n">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="H683" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I683" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M683" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A684" s="1" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B684" s="1" t="s">
-        <v>704</v>
+        <v>742</v>
       </c>
       <c r="C684" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F684" s="1" t="n">
-        <v>295</v>
+        <v>2292</v>
       </c>
       <c r="G684" s="1" t="n">
-        <v>124</v>
+        <v>3931</v>
       </c>
       <c r="H684" s="1" t="n">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="I684" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="J684" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="K684" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="L684" s="1" t="n">
+        <v>7</v>
+      </c>
       <c r="M684" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="N684" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="O684" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A685" s="1" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="B685" s="1" t="s">
         <v>742</v>
@@ -22662,39 +22695,39 @@
         <v>17</v>
       </c>
       <c r="F685" s="1" t="n">
-        <v>2292</v>
+        <v>1232</v>
       </c>
       <c r="G685" s="1" t="n">
-        <v>3931</v>
+        <v>792</v>
       </c>
       <c r="H685" s="1" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="I685" s="1" t="n">
-        <v>129</v>
+        <v>54</v>
       </c>
       <c r="J685" s="1" t="n">
         <v>34</v>
       </c>
       <c r="K685" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="L685" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="L685" s="1" t="n">
-        <v>7</v>
-      </c>
       <c r="M685" s="1" t="n">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="N685" s="1" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O685" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A686" s="1" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B686" s="1" t="s">
         <v>742</v>
@@ -22703,80 +22736,50 @@
         <v>17</v>
       </c>
       <c r="F686" s="1" t="n">
-        <v>1232</v>
+        <v>1472</v>
       </c>
       <c r="G686" s="1" t="n">
-        <v>792</v>
+        <v>593</v>
       </c>
       <c r="H686" s="1" t="n">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="I686" s="1" t="n">
-        <v>54</v>
+        <v>139</v>
       </c>
       <c r="J686" s="1" t="n">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="K686" s="1" t="n">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="L686" s="1" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="M686" s="1" t="n">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="N686" s="1" t="n">
         <v>2</v>
       </c>
       <c r="O686" s="1" t="n">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A687" s="1" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B687" s="1" t="s">
         <v>742</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F687" s="1" t="n">
-        <v>1472</v>
-      </c>
-      <c r="G687" s="1" t="n">
-        <v>593</v>
-      </c>
-      <c r="H687" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="I687" s="1" t="n">
-        <v>139</v>
-      </c>
-      <c r="J687" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="K687" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="L687" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="M687" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="N687" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="O687" s="1" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="1" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B688" s="1" t="s">
         <v>742</v>
@@ -22784,10 +22787,25 @@
       <c r="C688" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F688" s="1" t="n">
+        <v>1096</v>
+      </c>
+      <c r="G688" s="1" t="n">
+        <v>501</v>
+      </c>
+      <c r="H688" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="I688" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="M688" s="1" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A689" s="1" t="s">
-        <v>746</v>
+        <v>419</v>
       </c>
       <c r="B689" s="1" t="s">
         <v>742</v>
@@ -22796,50 +22814,53 @@
         <v>23</v>
       </c>
       <c r="F689" s="1" t="n">
-        <v>1096</v>
+        <v>88</v>
       </c>
       <c r="G689" s="1" t="n">
-        <v>501</v>
+        <v>17</v>
       </c>
       <c r="H689" s="1" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I689" s="1" t="n">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="M689" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A690" s="1" t="s">
-        <v>419</v>
+        <v>747</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>742</v>
+        <v>748</v>
       </c>
       <c r="C690" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D690" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="F690" s="1" t="n">
-        <v>88</v>
+        <v>5</v>
       </c>
       <c r="G690" s="1" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H690" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I690" s="1" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M690" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A691" s="1" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="B691" s="1" t="s">
         <v>748</v>
@@ -22847,28 +22868,25 @@
       <c r="C691" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D691" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F691" s="1" t="n">
-        <v>5</v>
+        <v>164</v>
       </c>
       <c r="G691" s="1" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="H691" s="1" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="I691" s="1" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="M691" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A692" s="1" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B692" s="1" t="s">
         <v>748</v>
@@ -22877,24 +22895,24 @@
         <v>23</v>
       </c>
       <c r="F692" s="1" t="n">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="G692" s="1" t="n">
-        <v>43</v>
+        <v>112</v>
       </c>
       <c r="H692" s="1" t="n">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="I692" s="1" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="M692" s="1" t="n">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A693" s="1" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B693" s="1" t="s">
         <v>748</v>
@@ -22903,16 +22921,16 @@
         <v>23</v>
       </c>
       <c r="F693" s="1" t="n">
-        <v>155</v>
+        <v>59</v>
       </c>
       <c r="G693" s="1" t="n">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="H693" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I693" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M693" s="1" t="n">
         <v>2</v>
@@ -22920,132 +22938,117 @@
     </row>
     <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A694" s="1" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B694" s="1" t="s">
         <v>748</v>
       </c>
       <c r="C694" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F694" s="1" t="n">
-        <v>59</v>
+        <v>1030</v>
       </c>
       <c r="G694" s="1" t="n">
-        <v>37</v>
+        <v>480</v>
       </c>
       <c r="H694" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I694" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="J694" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="K694" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L694" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="M694" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="N694" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A695" s="1" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B695" s="1" t="s">
-        <v>748</v>
+        <v>754</v>
       </c>
       <c r="C695" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F695" s="1" t="n">
-        <v>1030</v>
+        <v>128</v>
       </c>
       <c r="G695" s="1" t="n">
-        <v>480</v>
+        <v>34</v>
       </c>
       <c r="H695" s="1" t="n">
         <v>10</v>
       </c>
       <c r="I695" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="J695" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="K695" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L695" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M695" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="N695" s="1" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A696" s="1" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="B696" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C696" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F696" s="1" t="n">
-        <v>128</v>
+        <v>691</v>
       </c>
       <c r="G696" s="1" t="n">
-        <v>34</v>
+        <v>167</v>
       </c>
       <c r="H696" s="1" t="n">
         <v>10</v>
       </c>
       <c r="I696" s="1" t="n">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="J696" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="K696" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="M696" s="1" t="n">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="N696" s="1" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A697" s="1" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B697" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C697" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F697" s="1" t="n">
-        <v>691</v>
-      </c>
-      <c r="G697" s="1" t="n">
-        <v>167</v>
-      </c>
-      <c r="H697" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="I697" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="J697" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="K697" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M697" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N697" s="1" t="n">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A698" s="1" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B698" s="1" t="s">
         <v>754</v>
@@ -23053,77 +23056,92 @@
       <c r="C698" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F698" s="1" t="n">
+        <v>239</v>
+      </c>
+      <c r="G698" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="H698" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I698" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="M698" s="1" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A699" s="1" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B699" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C699" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F699" s="1" t="n">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="G699" s="1" t="n">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="H699" s="1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I699" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="J699" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="K699" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="L699" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="M699" s="1" t="n">
-        <v>17</v>
+        <v>3</v>
+      </c>
+      <c r="N699" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O699" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A700" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B700" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C700" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F700" s="1" t="n">
-        <v>211</v>
+        <v>912</v>
       </c>
       <c r="G700" s="1" t="n">
-        <v>135</v>
+        <v>466</v>
       </c>
       <c r="H700" s="1" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="I700" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J700" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="K700" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="L700" s="1" t="n">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="M700" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="N700" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="O700" s="1" t="n">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A701" s="1" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B701" s="1" t="s">
         <v>754</v>
@@ -23132,24 +23150,24 @@
         <v>23</v>
       </c>
       <c r="F701" s="1" t="n">
-        <v>912</v>
+        <v>574</v>
       </c>
       <c r="G701" s="1" t="n">
-        <v>466</v>
+        <v>0</v>
       </c>
       <c r="H701" s="1" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="I701" s="1" t="n">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="M701" s="1" t="n">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A702" s="1" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B702" s="1" t="s">
         <v>754</v>
@@ -23158,24 +23176,24 @@
         <v>23</v>
       </c>
       <c r="F702" s="1" t="n">
-        <v>574</v>
+        <v>54</v>
       </c>
       <c r="G702" s="1" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="H702" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I702" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M702" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A703" s="1" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B703" s="1" t="s">
         <v>754</v>
@@ -23183,25 +23201,10 @@
       <c r="C703" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F703" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="G703" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="H703" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I703" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="M703" s="1" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A704" s="1" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B704" s="1" t="s">
         <v>754</v>
@@ -23209,10 +23212,25 @@
       <c r="C704" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F704" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="G704" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="H704" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I704" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="M704" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A705" s="1" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B705" s="1" t="s">
         <v>754</v>
@@ -23221,16 +23239,16 @@
         <v>23</v>
       </c>
       <c r="F705" s="1" t="n">
-        <v>111</v>
+        <v>198</v>
       </c>
       <c r="G705" s="1" t="n">
-        <v>75</v>
+        <v>234</v>
       </c>
       <c r="H705" s="1" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I705" s="1" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="M705" s="1" t="n">
         <v>1</v>
@@ -23238,74 +23256,74 @@
     </row>
     <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A706" s="1" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B706" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C706" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F706" s="1" t="n">
-        <v>198</v>
+        <v>1214</v>
       </c>
       <c r="G706" s="1" t="n">
-        <v>234</v>
+        <v>390</v>
       </c>
       <c r="H706" s="1" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="I706" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="J706" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="K706" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="L706" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M706" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="N706" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="O706" s="1" t="n">
         <v>4</v>
-      </c>
-      <c r="M706" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A707" s="1" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B707" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C707" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F707" s="1" t="n">
-        <v>1214</v>
+        <v>208</v>
       </c>
       <c r="G707" s="1" t="n">
-        <v>390</v>
+        <v>154</v>
       </c>
       <c r="H707" s="1" t="n">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="I707" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="J707" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="K707" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="L707" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="M707" s="1" t="n">
         <v>11</v>
-      </c>
-      <c r="M707" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="N707" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="O707" s="1" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A708" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B708" s="1" t="s">
         <v>754</v>
@@ -23314,24 +23332,24 @@
         <v>23</v>
       </c>
       <c r="F708" s="1" t="n">
-        <v>208</v>
+        <v>73</v>
       </c>
       <c r="G708" s="1" t="n">
-        <v>154</v>
+        <v>0</v>
       </c>
       <c r="H708" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I708" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="M708" s="1" t="n">
         <v>3</v>
-      </c>
-      <c r="I708" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="M708" s="1" t="n">
-        <v>11</v>
       </c>
     </row>
     <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A709" s="1" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B709" s="1" t="s">
         <v>754</v>
@@ -23340,24 +23358,24 @@
         <v>23</v>
       </c>
       <c r="F709" s="1" t="n">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="G709" s="1" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H709" s="1" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="I709" s="1" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="M709" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A710" s="1" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B710" s="1" t="s">
         <v>754</v>
@@ -23366,24 +23384,24 @@
         <v>23</v>
       </c>
       <c r="F710" s="1" t="n">
-        <v>62</v>
+        <v>151</v>
       </c>
       <c r="G710" s="1" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="H710" s="1" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="I710" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M710" s="1" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A711" s="1" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B711" s="1" t="s">
         <v>754</v>
@@ -23392,24 +23410,24 @@
         <v>23</v>
       </c>
       <c r="F711" s="1" t="n">
-        <v>151</v>
+        <v>81</v>
       </c>
       <c r="G711" s="1" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H711" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="I711" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="I711" s="1" t="n">
-        <v>11</v>
-      </c>
       <c r="M711" s="1" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A712" s="1" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="B712" s="1" t="s">
         <v>754</v>
@@ -23417,109 +23435,124 @@
       <c r="C712" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F712" s="1" t="n">
-        <v>81</v>
-      </c>
-      <c r="G712" s="1" t="n">
-        <v>23</v>
-      </c>
       <c r="H712" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I712" s="1" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="M712" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A713" s="1" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="B713" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C713" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
+      </c>
+      <c r="F713" s="1" t="n">
+        <v>3080</v>
+      </c>
+      <c r="G713" s="1" t="n">
+        <v>2638</v>
       </c>
       <c r="H713" s="1" t="n">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="I713" s="1" t="n">
-        <v>1</v>
+        <v>64</v>
+      </c>
+      <c r="J713" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="K713" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L713" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="M713" s="1" t="n">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="N713" s="1" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A714" s="1" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="B714" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C714" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F714" s="1" t="n">
-        <v>3080</v>
+        <v>219</v>
       </c>
       <c r="G714" s="1" t="n">
-        <v>2638</v>
+        <v>39</v>
       </c>
       <c r="H714" s="1" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="I714" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="J714" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="K714" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="L714" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M714" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="N714" s="1" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A715" s="1" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B715" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C715" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F715" s="1" t="n">
-        <v>219</v>
+        <v>3286</v>
       </c>
       <c r="G715" s="1" t="n">
-        <v>39</v>
+        <v>629</v>
       </c>
       <c r="H715" s="1" t="n">
-        <v>10</v>
+        <v>73</v>
       </c>
       <c r="I715" s="1" t="n">
-        <v>8</v>
+        <v>51</v>
+      </c>
+      <c r="J715" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="K715" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="L715" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="M715" s="1" t="n">
-        <v>7</v>
+        <v>42</v>
+      </c>
+      <c r="N715" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="O715" s="1" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A716" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B716" s="1" t="s">
         <v>754</v>
@@ -23527,151 +23560,136 @@
       <c r="C716" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D716" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F716" s="1" t="n">
-        <v>3286</v>
+        <v>1772</v>
       </c>
       <c r="G716" s="1" t="n">
-        <v>629</v>
+        <v>0</v>
       </c>
       <c r="H716" s="1" t="n">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="I716" s="1" t="n">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="J716" s="1" t="n">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="K716" s="1" t="n">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="L716" s="1" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="M716" s="1" t="n">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="N716" s="1" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="O716" s="1" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A717" s="1" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B717" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C717" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D717" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F717" s="1" t="n">
-        <v>1772</v>
+        <v>102</v>
       </c>
       <c r="G717" s="1" t="n">
         <v>0</v>
       </c>
       <c r="H717" s="1" t="n">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="I717" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="J717" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="K717" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="L717" s="1" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="M717" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="N717" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="O717" s="1" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A718" s="1" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B718" s="1" t="s">
         <v>754</v>
       </c>
       <c r="C718" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F718" s="1" t="n">
-        <v>102</v>
+        <v>486</v>
       </c>
       <c r="G718" s="1" t="n">
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="H718" s="1" t="n">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="I718" s="1" t="n">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="J718" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="K718" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="L718" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="M718" s="1" t="n">
-        <v>5</v>
+        <v>30</v>
+      </c>
+      <c r="N718" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="O718" s="1" t="n">
+        <v>14</v>
       </c>
     </row>
     <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A719" s="1" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B719" s="1" t="s">
-        <v>754</v>
+        <v>779</v>
       </c>
       <c r="C719" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F719" s="1" t="n">
-        <v>486</v>
+        <v>426</v>
       </c>
       <c r="G719" s="1" t="n">
-        <v>316</v>
+        <v>194</v>
       </c>
       <c r="H719" s="1" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I719" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="J719" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="K719" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="L719" s="1" t="n">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="M719" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="N719" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="O719" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A720" s="1" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="B720" s="1" t="s">
         <v>779</v>
@@ -23680,24 +23698,24 @@
         <v>23</v>
       </c>
       <c r="F720" s="1" t="n">
-        <v>426</v>
+        <v>366</v>
       </c>
       <c r="G720" s="1" t="n">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="H720" s="1" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="I720" s="1" t="n">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="M720" s="1" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A721" s="1" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B721" s="1" t="s">
         <v>779</v>
@@ -23706,24 +23724,24 @@
         <v>23</v>
       </c>
       <c r="F721" s="1" t="n">
-        <v>366</v>
+        <v>450</v>
       </c>
       <c r="G721" s="1" t="n">
-        <v>169</v>
+        <v>88</v>
       </c>
       <c r="H721" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I721" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M721" s="1" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A722" s="1" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B722" s="1" t="s">
         <v>779</v>
@@ -23731,25 +23749,10 @@
       <c r="C722" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F722" s="1" t="n">
-        <v>450</v>
-      </c>
-      <c r="G722" s="1" t="n">
-        <v>88</v>
-      </c>
-      <c r="H722" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I722" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M722" s="1" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A723" s="1" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B723" s="1" t="s">
         <v>779</v>
@@ -23757,10 +23760,25 @@
       <c r="C723" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F723" s="1" t="n">
+        <v>319</v>
+      </c>
+      <c r="G723" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="H723" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="I723" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M723" s="1" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A724" s="1" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B724" s="1" t="s">
         <v>779</v>
@@ -23768,25 +23786,10 @@
       <c r="C724" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F724" s="1" t="n">
-        <v>319</v>
-      </c>
-      <c r="G724" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="H724" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="I724" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="M724" s="1" t="n">
-        <v>14</v>
-      </c>
     </row>
     <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A725" s="1" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B725" s="1" t="s">
         <v>779</v>
@@ -23794,10 +23797,25 @@
       <c r="C725" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F725" s="1" t="n">
+        <v>282</v>
+      </c>
+      <c r="G725" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="H725" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="I725" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="M725" s="1" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A726" s="1" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B726" s="1" t="s">
         <v>779</v>
@@ -23806,50 +23824,35 @@
         <v>23</v>
       </c>
       <c r="F726" s="1" t="n">
-        <v>282</v>
+        <v>130</v>
       </c>
       <c r="G726" s="1" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="H726" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I726" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="M726" s="1" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A727" s="1" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B727" s="1" t="s">
         <v>779</v>
       </c>
       <c r="C727" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F727" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="G727" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H727" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="I727" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="M727" s="1" t="n">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A728" s="1" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B728" s="1" t="s">
         <v>779</v>
@@ -23857,54 +23860,69 @@
       <c r="C728" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D728" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F728" s="1" t="n">
+        <v>3336</v>
+      </c>
+      <c r="G728" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H728" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="I728" s="1" t="n">
+        <v>254</v>
+      </c>
+      <c r="J728" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="K728" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="L728" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="M728" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="N728" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="O728" s="1" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A729" s="1" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B729" s="1" t="s">
         <v>779</v>
       </c>
       <c r="C729" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D729" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F729" s="1" t="n">
-        <v>3336</v>
+        <v>1067</v>
       </c>
       <c r="G729" s="1" t="n">
-        <v>0</v>
+        <v>455</v>
       </c>
       <c r="H729" s="1" t="n">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="I729" s="1" t="n">
-        <v>254</v>
-      </c>
-      <c r="J729" s="1" t="n">
-        <v>197</v>
-      </c>
-      <c r="K729" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="L729" s="1" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="M729" s="1" t="n">
-        <v>135</v>
-      </c>
-      <c r="N729" s="1" t="n">
         <v>11</v>
-      </c>
-      <c r="O729" s="1" t="n">
-        <v>17</v>
       </c>
     </row>
     <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A730" s="1" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B730" s="1" t="s">
         <v>779</v>
@@ -23912,25 +23930,28 @@
       <c r="C730" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D730" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="F730" s="1" t="n">
-        <v>1067</v>
+        <v>131</v>
       </c>
       <c r="G730" s="1" t="n">
-        <v>455</v>
+        <v>0</v>
       </c>
       <c r="H730" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I730" s="1" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="M730" s="1" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A731" s="1" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B731" s="1" t="s">
         <v>779</v>
@@ -23938,106 +23959,103 @@
       <c r="C731" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D731" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F731" s="1" t="n">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="G731" s="1" t="n">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="H731" s="1" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="I731" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M731" s="1" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A732" s="1" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B732" s="1" t="s">
-        <v>779</v>
+        <v>793</v>
       </c>
       <c r="C732" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F732" s="1" t="n">
-        <v>118</v>
-      </c>
-      <c r="G732" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="H732" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="I732" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="M732" s="1" t="n">
-        <v>25</v>
       </c>
     </row>
     <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A733" s="1" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="B733" s="1" t="s">
         <v>793</v>
       </c>
       <c r="C733" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="F733" s="1" t="n">
+        <v>1895</v>
+      </c>
+      <c r="G733" s="1" t="n">
+        <v>672</v>
+      </c>
+      <c r="H733" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="I733" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="J733" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="K733" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="L733" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="M733" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="N733" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="O733" s="1" t="n">
+        <v>11</v>
       </c>
     </row>
     <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A734" s="1" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="B734" s="1" t="s">
         <v>793</v>
       </c>
       <c r="C734" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F734" s="1" t="n">
-        <v>1895</v>
+        <v>198</v>
       </c>
       <c r="G734" s="1" t="n">
-        <v>672</v>
+        <v>59</v>
       </c>
       <c r="H734" s="1" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I734" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="J734" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="K734" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="L734" s="1" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="M734" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="N734" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="O734" s="1" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A735" s="1" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B735" s="1" t="s">
         <v>793</v>
@@ -24045,36 +24063,36 @@
       <c r="C735" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F735" s="1" t="n">
-        <v>198</v>
-      </c>
-      <c r="G735" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="H735" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="I735" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="M735" s="1" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A736" s="1" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B736" s="1" t="s">
-        <v>793</v>
+        <v>798</v>
       </c>
       <c r="C736" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="F736" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="G736" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H736" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="I736" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="M736" s="1" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A737" s="1" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="B737" s="1" t="s">
         <v>798</v>
@@ -24083,24 +24101,24 @@
         <v>23</v>
       </c>
       <c r="F737" s="1" t="n">
-        <v>67</v>
+        <v>194</v>
       </c>
       <c r="G737" s="1" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="H737" s="1" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I737" s="1" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="M737" s="1" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A738" s="1" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="B738" s="1" t="s">
         <v>798</v>
@@ -24109,16 +24127,16 @@
         <v>23</v>
       </c>
       <c r="F738" s="1" t="n">
-        <v>194</v>
+        <v>124</v>
       </c>
       <c r="G738" s="1" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H738" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I738" s="1" t="n">
         <v>11</v>
-      </c>
-      <c r="I738" s="1" t="n">
-        <v>15</v>
       </c>
       <c r="M738" s="1" t="n">
         <v>10</v>
@@ -24126,7 +24144,7 @@
     </row>
     <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A739" s="1" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="B739" s="1" t="s">
         <v>798</v>
@@ -24135,24 +24153,24 @@
         <v>23</v>
       </c>
       <c r="F739" s="1" t="n">
-        <v>124</v>
+        <v>569</v>
       </c>
       <c r="G739" s="1" t="n">
-        <v>0</v>
+        <v>154</v>
       </c>
       <c r="H739" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I739" s="1" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="M739" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A740" s="1" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="B740" s="1" t="s">
         <v>798</v>
@@ -24161,24 +24179,24 @@
         <v>23</v>
       </c>
       <c r="F740" s="1" t="n">
-        <v>569</v>
+        <v>59</v>
       </c>
       <c r="G740" s="1" t="n">
-        <v>154</v>
+        <v>55</v>
       </c>
       <c r="H740" s="1" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I740" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M740" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A741" s="1" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B741" s="1" t="s">
         <v>798</v>
@@ -24187,24 +24205,24 @@
         <v>23</v>
       </c>
       <c r="F741" s="1" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="G741" s="1" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="H741" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="I741" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="M741" s="1" t="n">
         <v>2</v>
-      </c>
-      <c r="I741" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="M741" s="1" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A742" s="1" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B742" s="1" t="s">
         <v>798</v>
@@ -24213,24 +24231,24 @@
         <v>23</v>
       </c>
       <c r="F742" s="1" t="n">
-        <v>62</v>
+        <v>609</v>
       </c>
       <c r="G742" s="1" t="n">
-        <v>0</v>
+        <v>746</v>
       </c>
       <c r="H742" s="1" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="I742" s="1" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="M742" s="1" t="n">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A743" s="1" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B743" s="1" t="s">
         <v>798</v>
@@ -24239,50 +24257,68 @@
         <v>23</v>
       </c>
       <c r="F743" s="1" t="n">
-        <v>609</v>
+        <v>816</v>
       </c>
       <c r="G743" s="1" t="n">
-        <v>746</v>
+        <v>264</v>
       </c>
       <c r="H743" s="1" t="n">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="I743" s="1" t="n">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="M743" s="1" t="n">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A744" s="1" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B744" s="1" t="s">
         <v>798</v>
       </c>
       <c r="C744" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="D744" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="F744" s="1" t="n">
-        <v>816</v>
+        <v>3271</v>
       </c>
       <c r="G744" s="1" t="n">
-        <v>264</v>
+        <v>0</v>
       </c>
       <c r="H744" s="1" t="n">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="I744" s="1" t="n">
-        <v>50</v>
+        <v>89</v>
+      </c>
+      <c r="J744" s="1" t="n">
+        <v>185</v>
+      </c>
+      <c r="K744" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="L744" s="1" t="n">
+        <v>39</v>
       </c>
       <c r="M744" s="1" t="n">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="N744" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="O744" s="1" t="n">
+        <v>16</v>
       </c>
     </row>
     <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A745" s="1" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B745" s="1" t="s">
         <v>798</v>
@@ -24290,84 +24326,66 @@
       <c r="C745" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D745" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F745" s="1" t="n">
-        <v>3271</v>
+        <v>1882</v>
       </c>
       <c r="G745" s="1" t="n">
-        <v>0</v>
+        <v>786</v>
       </c>
       <c r="H745" s="1" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I745" s="1" t="n">
-        <v>89</v>
+        <v>13</v>
       </c>
       <c r="J745" s="1" t="n">
-        <v>185</v>
+        <v>46</v>
       </c>
       <c r="K745" s="1" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="L745" s="1" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="M745" s="1" t="n">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="N745" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O745" s="1" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A746" s="1" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B746" s="1" t="s">
         <v>798</v>
       </c>
       <c r="C746" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F746" s="1" t="n">
-        <v>1882</v>
+        <v>181</v>
       </c>
       <c r="G746" s="1" t="n">
-        <v>786</v>
+        <v>259</v>
       </c>
       <c r="H746" s="1" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I746" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="J746" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="K746" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="L746" s="1" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M746" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="N746" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="O746" s="1" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A747" s="1" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B747" s="1" t="s">
         <v>798</v>
@@ -24376,24 +24394,21 @@
         <v>23</v>
       </c>
       <c r="F747" s="1" t="n">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="G747" s="1" t="n">
-        <v>259</v>
+        <v>36</v>
       </c>
       <c r="H747" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="I747" s="1" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="M747" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A748" s="1" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B748" s="1" t="s">
         <v>798</v>
@@ -24402,21 +24417,24 @@
         <v>23</v>
       </c>
       <c r="F748" s="1" t="n">
-        <v>150</v>
+        <v>373</v>
       </c>
       <c r="G748" s="1" t="n">
-        <v>36</v>
+        <v>342</v>
       </c>
       <c r="H748" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="I748" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="M748" s="1" t="n">
         <v>16</v>
-      </c>
-      <c r="M748" s="1" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A749" s="1" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B749" s="1" t="s">
         <v>798</v>
@@ -24425,24 +24443,24 @@
         <v>23</v>
       </c>
       <c r="F749" s="1" t="n">
-        <v>373</v>
+        <v>533</v>
       </c>
       <c r="G749" s="1" t="n">
-        <v>342</v>
+        <v>486</v>
       </c>
       <c r="H749" s="1" t="n">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="I749" s="1" t="n">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="M749" s="1" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A750" s="1" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B750" s="1" t="s">
         <v>798</v>
@@ -24451,91 +24469,66 @@
         <v>23</v>
       </c>
       <c r="F750" s="1" t="n">
-        <v>533</v>
+        <v>395</v>
       </c>
       <c r="G750" s="1" t="n">
-        <v>486</v>
+        <v>105</v>
       </c>
       <c r="H750" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I750" s="1" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M750" s="1" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A751" s="1" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B751" s="1" t="s">
-        <v>798</v>
+        <v>814</v>
       </c>
       <c r="C751" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
+      </c>
+      <c r="D751" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="F751" s="1" t="n">
-        <v>395</v>
+        <v>424</v>
       </c>
       <c r="G751" s="1" t="n">
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="H751" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I751" s="1" t="n">
-        <v>17</v>
+        <v>11</v>
+      </c>
+      <c r="J751" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="K751" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="L751" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="M751" s="1" t="n">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A752" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="B752" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="C752" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D752" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F752" s="1" t="n">
-        <v>424</v>
-      </c>
-      <c r="G752" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H752" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="I752" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="J752" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="K752" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="L752" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="M752" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="N752" s="1" t="n">
+      <c r="N751" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="O752" s="1" t="n">
+      <c r="O751" s="1" t="n">
         <v>1</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>